<commit_message>
included dictt-to-dataframe and csv-to-dataframe
</commit_message>
<xml_diff>
--- a/random_numbers_with_xlwriter_output.xlsx
+++ b/random_numbers_with_xlwriter_output.xlsx
@@ -386,10 +386,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.03720948872797411</v>
+        <v>0.3612576861019183</v>
       </c>
       <c r="C2">
-        <v>1.309323401952467</v>
+        <v>-0.4509741943077296</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -397,10 +397,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.3919986754883391</v>
+        <v>1.072760912955931</v>
       </c>
       <c r="C3">
-        <v>0.06517309704026636</v>
+        <v>1.323403035260815</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -408,10 +408,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.834090223488112</v>
+        <v>-2.223533206927786</v>
       </c>
       <c r="C4">
-        <v>-0.01938098207905093</v>
+        <v>-2.014220626320781</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -419,10 +419,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.2538281173378009</v>
+        <v>-0.4541552108325183</v>
       </c>
       <c r="C5">
-        <v>1.138400121767726</v>
+        <v>-1.470128849536629</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -430,10 +430,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.1103743146428517</v>
+        <v>0.04363076571425182</v>
       </c>
       <c r="C6">
-        <v>0.3370405326580067</v>
+        <v>1.31548766476951</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -441,10 +441,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.5093420689633096</v>
+        <v>0.5573719852671605</v>
       </c>
       <c r="C7">
-        <v>0.7964385857600206</v>
+        <v>0.985233437181221</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -452,10 +452,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5980531184122375</v>
+        <v>1.356332413291238</v>
       </c>
       <c r="C8">
-        <v>-0.6450768623091623</v>
+        <v>-0.8306242058244614</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -463,10 +463,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1.00608700684404</v>
+        <v>1.273320796424101</v>
       </c>
       <c r="C9">
-        <v>-0.603348453286611</v>
+        <v>-0.1623508622203794</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -474,10 +474,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.4933411906263996</v>
+        <v>1.921523992568382</v>
       </c>
       <c r="C10">
-        <v>-0.123724114912895</v>
+        <v>-0.1545241888779368</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -485,10 +485,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.876998787656914</v>
+        <v>-1.25789201893243</v>
       </c>
       <c r="C11">
-        <v>0.2035298003491941</v>
+        <v>0.1769685652705896</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -496,10 +496,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.7047834155261721</v>
+        <v>0.09143695731503515</v>
       </c>
       <c r="C12">
-        <v>-0.07543595556137457</v>
+        <v>-0.762360619456082</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -507,10 +507,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.528756566945941</v>
+        <v>1.263500159971155</v>
       </c>
       <c r="C13">
-        <v>-0.2164981443028435</v>
+        <v>1.857740028936024</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -518,10 +518,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-1.672506114866705</v>
+        <v>-1.577816169294582</v>
       </c>
       <c r="C14">
-        <v>-0.4466793277456049</v>
+        <v>0.6835528390940024</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -529,10 +529,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.2771877959551278</v>
+        <v>-1.45541334951761</v>
       </c>
       <c r="C15">
-        <v>-1.543711665226544</v>
+        <v>1.156616098024375</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -540,10 +540,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.2446433101150768</v>
+        <v>0.7105966832944799</v>
       </c>
       <c r="C16">
-        <v>0.5628251183764351</v>
+        <v>1.125894238764907</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -551,10 +551,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.6859398532260532</v>
+        <v>2.218016733655032</v>
       </c>
       <c r="C17">
-        <v>-0.4475179281360587</v>
+        <v>0.2757083563123999</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -562,10 +562,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.3304955583844395</v>
+        <v>-0.6817645475159038</v>
       </c>
       <c r="C18">
-        <v>-0.164550969455649</v>
+        <v>-0.3416254152425416</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -573,10 +573,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.7424070047258208</v>
+        <v>-0.27493338232481</v>
       </c>
       <c r="C19">
-        <v>-0.2190361768235021</v>
+        <v>1.335834918543516</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -584,10 +584,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.1400681440730674</v>
+        <v>-0.8486038256819711</v>
       </c>
       <c r="C20">
-        <v>-0.2424397902358672</v>
+        <v>-0.6355365040560987</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -595,10 +595,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-1.516106163002395</v>
+        <v>0.1795837068335649</v>
       </c>
       <c r="C21">
-        <v>1.219611964926717</v>
+        <v>0.232123768427802</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -606,10 +606,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-0.3502479021381502</v>
+        <v>-0.5910124643022954</v>
       </c>
       <c r="C22">
-        <v>0.3250619193224238</v>
+        <v>-0.5721863496283152</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -617,10 +617,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.2586011461885713</v>
+        <v>-1.165204771974269</v>
       </c>
       <c r="C23">
-        <v>0.2063697510729293</v>
+        <v>-0.4868852690078531</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -628,10 +628,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.39946275015918</v>
+        <v>0.7544531792817407</v>
       </c>
       <c r="C24">
-        <v>-0.004706383078521205</v>
+        <v>1.160976745851848</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -639,10 +639,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2.006992790028144</v>
+        <v>-0.1291872541013901</v>
       </c>
       <c r="C25">
-        <v>1.049953848688059</v>
+        <v>-0.04034992892282423</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -650,10 +650,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.07822579435052127</v>
+        <v>-0.8425278541924752</v>
       </c>
       <c r="C26">
-        <v>-0.4701748682762957</v>
+        <v>-0.9305465810992486</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -661,10 +661,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-1.633131032255829</v>
+        <v>0.5058555067886076</v>
       </c>
       <c r="C27">
-        <v>-1.613072470413365</v>
+        <v>-1.241718454890224</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -672,10 +672,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.04053225265468481</v>
+        <v>-0.6100046258041366</v>
       </c>
       <c r="C28">
-        <v>0.8537510904100087</v>
+        <v>0.4525099422651947</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -683,10 +683,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-0.1048567389553055</v>
+        <v>-0.1509779960897119</v>
       </c>
       <c r="C29">
-        <v>-0.3773313989721249</v>
+        <v>-0.4423193269248121</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -694,10 +694,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2.076210878530794</v>
+        <v>-0.7421991892472307</v>
       </c>
       <c r="C30">
-        <v>0.3535516795127387</v>
+        <v>0.2847661705101655</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -705,10 +705,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-1.405092291047453</v>
+        <v>0.2804545970828457</v>
       </c>
       <c r="C31">
-        <v>-1.309638423477404</v>
+        <v>0.9321358610322161</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -716,10 +716,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.8935721101564066</v>
+        <v>-0.8787503483256203</v>
       </c>
       <c r="C32">
-        <v>-0.1830294807588949</v>
+        <v>0.8894581796848809</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -727,10 +727,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-0.3816243214237293</v>
+        <v>-0.05591412642934081</v>
       </c>
       <c r="C33">
-        <v>-2.502313772311484</v>
+        <v>-0.6280738252289281</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -738,10 +738,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-1.1982627390895</v>
+        <v>1.475409121465419</v>
       </c>
       <c r="C34">
-        <v>-0.9365932478562008</v>
+        <v>-3.712209086132272</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -749,10 +749,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.3684379821348343</v>
+        <v>1.432567321104183</v>
       </c>
       <c r="C35">
-        <v>-0.1214274146370679</v>
+        <v>-1.275052558074382</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -760,10 +760,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-0.1652659623795506</v>
+        <v>0.8313185647595208</v>
       </c>
       <c r="C36">
-        <v>0.1922739087044662</v>
+        <v>-0.6117430478060771</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -771,10 +771,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.6337269366711432</v>
+        <v>-0.3756477064979983</v>
       </c>
       <c r="C37">
-        <v>-1.547423585420839</v>
+        <v>0.4507872800818774</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -782,10 +782,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.4610968535917163</v>
+        <v>1.262201538123624</v>
       </c>
       <c r="C38">
-        <v>-1.331044487737021</v>
+        <v>0.500512945526479</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -793,10 +793,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1.725094199082794</v>
+        <v>-0.07687390305110446</v>
       </c>
       <c r="C39">
-        <v>-1.17161293181069</v>
+        <v>-1.317246099328447</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -804,10 +804,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>-0.9037643352422333</v>
+        <v>-0.344341875036944</v>
       </c>
       <c r="C40">
-        <v>-0.7372390890326799</v>
+        <v>0.7556265496813992</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -815,10 +815,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.9859646787837105</v>
+        <v>0.03240034865184849</v>
       </c>
       <c r="C41">
-        <v>-1.432295842600209</v>
+        <v>0.7051514399887938</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -826,10 +826,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.1865166562755004</v>
+        <v>1.359152849973659</v>
       </c>
       <c r="C42">
-        <v>0.2230102239949709</v>
+        <v>-1.765596695700185</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -837,10 +837,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-0.7971401887734428</v>
+        <v>-0.4009145537477865</v>
       </c>
       <c r="C43">
-        <v>-0.4805254438852702</v>
+        <v>0.1840956780260982</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -848,10 +848,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-0.9934495926907041</v>
+        <v>-1.630099515024667</v>
       </c>
       <c r="C44">
-        <v>-2.118682369986959</v>
+        <v>0.6946797792283357</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -859,10 +859,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.4079958187520145</v>
+        <v>0.9916997209325101</v>
       </c>
       <c r="C45">
-        <v>-0.3430486237640827</v>
+        <v>-0.6492928904908877</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -870,10 +870,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>-1.528528118092924</v>
+        <v>-0.3206823915518093</v>
       </c>
       <c r="C46">
-        <v>-0.0238455808302033</v>
+        <v>0.7873452715395616</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -881,10 +881,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-0.1451522026575521</v>
+        <v>0.6391874134074733</v>
       </c>
       <c r="C47">
-        <v>-0.4687801118774245</v>
+        <v>-0.9575491450435945</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -892,10 +892,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.300558269465067</v>
+        <v>0.2897337558199167</v>
       </c>
       <c r="C48">
-        <v>-1.184554420884946</v>
+        <v>-0.5943673522018498</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -903,10 +903,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>1.038942738846851</v>
+        <v>-0.05421613005148891</v>
       </c>
       <c r="C49">
-        <v>-1.437215550880365</v>
+        <v>-0.7559319867919181</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -914,10 +914,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-0.4024608847595614</v>
+        <v>0.006279106908708441</v>
       </c>
       <c r="C50">
-        <v>-2.8180684876985</v>
+        <v>-1.082357608942842</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -925,10 +925,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-0.1802867221787775</v>
+        <v>-0.9747821915710172</v>
       </c>
       <c r="C51">
-        <v>0.5757181596138384</v>
+        <v>1.265827095820597</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -936,10 +936,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.3993657597427228</v>
+        <v>1.342666537906208</v>
       </c>
       <c r="C52">
-        <v>-0.1099734293567553</v>
+        <v>-1.249160017018655</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -947,10 +947,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.7460160527999034</v>
+        <v>0.1508419392006338</v>
       </c>
       <c r="C53">
-        <v>1.062929136122724</v>
+        <v>1.267987488945343</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -958,10 +958,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.3021540232114852</v>
+        <v>-1.535235235320922</v>
       </c>
       <c r="C54">
-        <v>0.5866165857250591</v>
+        <v>-0.3855958121579839</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -969,10 +969,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.958278243340834</v>
+        <v>2.415776914015987</v>
       </c>
       <c r="C55">
-        <v>0.6058224649476177</v>
+        <v>3.640151394197029</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -980,10 +980,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-1.200102956226536</v>
+        <v>0.09019799498806119</v>
       </c>
       <c r="C56">
-        <v>0.871798670008303</v>
+        <v>0.6270576958587428</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -991,10 +991,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>-1.015010959983729</v>
+        <v>-0.8540954032864616</v>
       </c>
       <c r="C57">
-        <v>0.01006810090984564</v>
+        <v>0.2413827670165126</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1002,10 +1002,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.3891865054848297</v>
+        <v>0.4374416388086468</v>
       </c>
       <c r="C58">
-        <v>-0.07742450464805826</v>
+        <v>0.1006986299289985</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1013,10 +1013,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-0.6981348860095365</v>
+        <v>-0.9233010094526276</v>
       </c>
       <c r="C59">
-        <v>0.3692605776381632</v>
+        <v>0.883215672730206</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1024,10 +1024,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.5129781382312647</v>
+        <v>-0.8999821962450502</v>
       </c>
       <c r="C60">
-        <v>-0.647135391344714</v>
+        <v>1.215670091254053</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1035,10 +1035,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>-0.7100372285129756</v>
+        <v>0.851753240375213</v>
       </c>
       <c r="C61">
-        <v>0.7445374093500802</v>
+        <v>0.6351474396423097</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1046,10 +1046,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.8070519826764188</v>
+        <v>0.7484689341607939</v>
       </c>
       <c r="C62">
-        <v>-1.756025957636049</v>
+        <v>0.5214220227073247</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1057,10 +1057,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>1.895205792300778</v>
+        <v>0.4935081156732377</v>
       </c>
       <c r="C63">
-        <v>-0.8548564703125</v>
+        <v>2.128450041800609</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1068,10 +1068,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.804273680679196</v>
+        <v>-0.03055186249477717</v>
       </c>
       <c r="C64">
-        <v>0.1113846508463748</v>
+        <v>-0.143797569597825</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1079,10 +1079,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>-0.006968311295869916</v>
+        <v>-1.159737680075293</v>
       </c>
       <c r="C65">
-        <v>0.8603791257088087</v>
+        <v>1.211727073251258</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1090,10 +1090,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-0.7932334797741554</v>
+        <v>1.955641840629737</v>
       </c>
       <c r="C66">
-        <v>0.1267359460327533</v>
+        <v>0.5158039181586543</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1101,10 +1101,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-1.289044582799864</v>
+        <v>-0.5615522813127793</v>
       </c>
       <c r="C67">
-        <v>-0.9134309607774472</v>
+        <v>-0.7321524595508115</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1112,10 +1112,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>-1.451088566410362</v>
+        <v>-1.252168502250617</v>
       </c>
       <c r="C68">
-        <v>1.524006104239222</v>
+        <v>-0.9108252794868594</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1123,10 +1123,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.5899457852356123</v>
+        <v>-0.9926511710365622</v>
       </c>
       <c r="C69">
-        <v>-0.5173373380225369</v>
+        <v>1.144612553394971</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1134,10 +1134,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.5921117970030341</v>
+        <v>-1.073982317310868</v>
       </c>
       <c r="C70">
-        <v>-0.6494513990088789</v>
+        <v>-1.088096258958459</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1145,10 +1145,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.3651196961604212</v>
+        <v>-0.1851652111700238</v>
       </c>
       <c r="C71">
-        <v>-0.4284658916356235</v>
+        <v>0.5468494203714616</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1156,10 +1156,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>-1.965863705442977</v>
+        <v>-1.49915082363527</v>
       </c>
       <c r="C72">
-        <v>2.344455343280827</v>
+        <v>-0.6895255737874011</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1167,10 +1167,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.7292498928692146</v>
+        <v>-0.6104732474361267</v>
       </c>
       <c r="C73">
-        <v>0.4062262318019188</v>
+        <v>-0.4789128477559996</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1178,10 +1178,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>-2.148380289548153</v>
+        <v>-0.4851243429616592</v>
       </c>
       <c r="C74">
-        <v>-1.574340660917961</v>
+        <v>-0.9967740784190157</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1189,10 +1189,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.2246411633094753</v>
+        <v>-0.6464803016285395</v>
       </c>
       <c r="C75">
-        <v>-1.150354843952479</v>
+        <v>0.5059481888541476</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1200,10 +1200,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.3048298292759475</v>
+        <v>-0.2412225223531705</v>
       </c>
       <c r="C76">
-        <v>-0.5714262685268321</v>
+        <v>-0.09851401685720333</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1211,10 +1211,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>-1.543251963868612</v>
+        <v>-0.7589771737214381</v>
       </c>
       <c r="C77">
-        <v>2.54307412245962</v>
+        <v>0.612809554523842</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1222,10 +1222,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>-0.05861549731892987</v>
+        <v>-1.504296638388803</v>
       </c>
       <c r="C78">
-        <v>1.124707654158492</v>
+        <v>0.4324245218038146</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1233,10 +1233,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>-0.8631824220161933</v>
+        <v>-0.2460990988316427</v>
       </c>
       <c r="C79">
-        <v>0.3406971534071732</v>
+        <v>-0.2305538338288785</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1244,10 +1244,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.3999943895185519</v>
+        <v>0.7024780289185819</v>
       </c>
       <c r="C80">
-        <v>-1.108219577472989</v>
+        <v>-0.1082448806498865</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1255,10 +1255,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-0.491602794849259</v>
+        <v>-0.3701255443416016</v>
       </c>
       <c r="C81">
-        <v>-1.054922086733921</v>
+        <v>1.614710020551191</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1266,10 +1266,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-1.686555733660987</v>
+        <v>0.6509274161316182</v>
       </c>
       <c r="C82">
-        <v>-0.7007356278561729</v>
+        <v>-0.8774883838271481</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1277,10 +1277,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-0.8866795111519928</v>
+        <v>1.965929578110975</v>
       </c>
       <c r="C83">
-        <v>0.2931878477268643</v>
+        <v>0.06149780411508734</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1288,10 +1288,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-0.06598212901062446</v>
+        <v>-1.124728687083829</v>
       </c>
       <c r="C84">
-        <v>0.4063001535329512</v>
+        <v>-0.5112364039459796</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1299,10 +1299,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.8423740162504197</v>
+        <v>-1.163967608764706</v>
       </c>
       <c r="C85">
-        <v>0.3294497852061493</v>
+        <v>-0.3317493472259974</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1310,10 +1310,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.8181770062999248</v>
+        <v>1.17192008538866</v>
       </c>
       <c r="C86">
-        <v>-1.621701122361456</v>
+        <v>-1.628158169329231</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1321,10 +1321,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>-2.397705090400355</v>
+        <v>-0.3409021238902183</v>
       </c>
       <c r="C87">
-        <v>0.6712830799234155</v>
+        <v>-0.8044972596044605</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1332,10 +1332,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.9218918297019979</v>
+        <v>-0.6725688848511649</v>
       </c>
       <c r="C88">
-        <v>-0.2622963738070497</v>
+        <v>-1.600808533454595</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1343,10 +1343,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>-0.286953138881795</v>
+        <v>-2.085134033459898</v>
       </c>
       <c r="C89">
-        <v>-0.3271892033048929</v>
+        <v>-0.04795870085326444</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1354,10 +1354,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>-0.1362662812985165</v>
+        <v>0.1412090957939897</v>
       </c>
       <c r="C90">
-        <v>1.153769026770374</v>
+        <v>0.3905611584724428</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1365,10 +1365,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.4081720723370555</v>
+        <v>0.6909871274527043</v>
       </c>
       <c r="C91">
-        <v>1.574587068579609</v>
+        <v>0.7547027560414153</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1376,10 +1376,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>2.100480180803781</v>
+        <v>-1.593648091970933</v>
       </c>
       <c r="C92">
-        <v>-0.4355758033867373</v>
+        <v>1.82945583946556</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1387,10 +1387,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.2741587376513458</v>
+        <v>0.930962100479273</v>
       </c>
       <c r="C93">
-        <v>1.681074441199979</v>
+        <v>0.331799236243687</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1398,10 +1398,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.1550643352149153</v>
+        <v>-1.33779385982084</v>
       </c>
       <c r="C94">
-        <v>0.9996451583213286</v>
+        <v>1.016912381781475</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1409,10 +1409,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.5472510359410462</v>
+        <v>0.2501472464414053</v>
       </c>
       <c r="C95">
-        <v>0.8823833871307372</v>
+        <v>-0.3899216185163425</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1420,10 +1420,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>-0.445206882896886</v>
+        <v>-0.813501982848896</v>
       </c>
       <c r="C96">
-        <v>0.2815049899029227</v>
+        <v>-0.806083392596592</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1431,10 +1431,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-1.408879834611319</v>
+        <v>1.755208447096476</v>
       </c>
       <c r="C97">
-        <v>-0.2725901098675195</v>
+        <v>-1.829610632654696</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1442,10 +1442,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.3103704902693449</v>
+        <v>-0.7069807519600606</v>
       </c>
       <c r="C98">
-        <v>-0.2069150468937817</v>
+        <v>0.5192920744534519</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1453,10 +1453,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>2.014223373482032</v>
+        <v>-1.923254508564905</v>
       </c>
       <c r="C99">
-        <v>1.245643189735796</v>
+        <v>-1.12854224711177</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1464,10 +1464,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.4140368059827885</v>
+        <v>0.3361507073238273</v>
       </c>
       <c r="C100">
-        <v>-1.88570446489045</v>
+        <v>-0.7746504858412326</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1475,10 +1475,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-1.381731742650687</v>
+        <v>0.265972173313786</v>
       </c>
       <c r="C101">
-        <v>0.06223003513892545</v>
+        <v>1.009115080395798</v>
       </c>
     </row>
   </sheetData>
@@ -1507,10 +1507,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8556734917647433</v>
+        <v>-0.3105346377330399</v>
       </c>
       <c r="C2">
-        <v>-0.02890123874558588</v>
+        <v>0.05413794446748554</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1518,10 +1518,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.004580121536094731</v>
+        <v>0.5302369519649347</v>
       </c>
       <c r="C3">
-        <v>-0.3046019389169655</v>
+        <v>1.023604089746236</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1529,10 +1529,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.408120580282276</v>
+        <v>-0.3147239913714737</v>
       </c>
       <c r="C4">
-        <v>-0.3295574643109213</v>
+        <v>-1.695282160566164</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1540,10 +1540,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.7203713896829403</v>
+        <v>-0.6394985134357829</v>
       </c>
       <c r="C5">
-        <v>2.587577127683153</v>
+        <v>-0.4998963695987991</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1551,10 +1551,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-2.031395707690953</v>
+        <v>0.3788442196684324</v>
       </c>
       <c r="C6">
-        <v>1.029597396078235</v>
+        <v>-0.9665091379656982</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1562,10 +1562,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-1.026078453649645</v>
+        <v>-0.08835473213005463</v>
       </c>
       <c r="C7">
-        <v>-0.9731211570201407</v>
+        <v>-0.5831593033059375</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1573,10 +1573,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.5641967954405858</v>
+        <v>0.1445391582816939</v>
       </c>
       <c r="C8">
-        <v>-0.0684153510036515</v>
+        <v>0.1894315089882786</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1584,10 +1584,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.4253363796643977</v>
+        <v>-0.6106681101487853</v>
       </c>
       <c r="C9">
-        <v>-1.316290040335153</v>
+        <v>0.93590113117422</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1595,10 +1595,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.8833199249010921</v>
+        <v>-1.082724536445241</v>
       </c>
       <c r="C10">
-        <v>-0.09968426165613158</v>
+        <v>1.846750269793585</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1606,10 +1606,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.9935581169052905</v>
+        <v>2.393906178139114</v>
       </c>
       <c r="C11">
-        <v>0.2539964657353627</v>
+        <v>1.048650369095102</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1617,10 +1617,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.4305113744639221</v>
+        <v>1.333680588244507</v>
       </c>
       <c r="C12">
-        <v>0.7985792627218552</v>
+        <v>0.1924785980312658</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1628,10 +1628,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-1.021150565880143</v>
+        <v>0.4270434751307727</v>
       </c>
       <c r="C13">
-        <v>0.02766866282041432</v>
+        <v>1.082913654666637</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1639,10 +1639,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.2023686510334629</v>
+        <v>0.3318992485700608</v>
       </c>
       <c r="C14">
-        <v>-2.092408697903179</v>
+        <v>-0.01876243590047583</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1650,10 +1650,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.3773362475704745</v>
+        <v>0.4251144345187799</v>
       </c>
       <c r="C15">
-        <v>-0.7940963382326949</v>
+        <v>0.4879156769374696</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1661,10 +1661,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2.932928675096794</v>
+        <v>0.4954357930324635</v>
       </c>
       <c r="C16">
-        <v>-1.270305105634506</v>
+        <v>0.3647759752077492</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1672,10 +1672,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.4995579079019577</v>
+        <v>0.08025189153805912</v>
       </c>
       <c r="C17">
-        <v>-0.8447863689270126</v>
+        <v>0.7556141739682873</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1683,10 +1683,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.9055165584819223</v>
+        <v>1.049154377482308</v>
       </c>
       <c r="C18">
-        <v>-0.1346779519256375</v>
+        <v>-0.1954352659640649</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1694,10 +1694,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-2.068547551653368</v>
+        <v>-0.07861347180143066</v>
       </c>
       <c r="C19">
-        <v>-0.2369605930502877</v>
+        <v>-0.7419153130682609</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1705,10 +1705,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-2.599926247203904</v>
+        <v>-1.391935024954457</v>
       </c>
       <c r="C20">
-        <v>-1.077065227667506</v>
+        <v>-1.778526639008862</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1716,10 +1716,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1.203996030205592</v>
+        <v>1.022248024335831</v>
       </c>
       <c r="C21">
-        <v>0.1615044535959827</v>
+        <v>0.8720867488142698</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1727,10 +1727,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-1.391247267147026</v>
+        <v>0.4844061906485407</v>
       </c>
       <c r="C22">
-        <v>0.7081741137329637</v>
+        <v>-1.003121344778884</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1738,10 +1738,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-0.5504183824042218</v>
+        <v>-0.1772686227894866</v>
       </c>
       <c r="C23">
-        <v>-1.507239347647985</v>
+        <v>-1.284668345576415</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1749,10 +1749,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.3974977977391428</v>
+        <v>0.1395888299273537</v>
       </c>
       <c r="C24">
-        <v>1.875498041152335</v>
+        <v>-0.5270875609555552</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1760,10 +1760,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.6730326407818338</v>
+        <v>0.1113553175756821</v>
       </c>
       <c r="C25">
-        <v>0.2148737864514857</v>
+        <v>0.07869917660029876</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1771,10 +1771,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-0.5652939507660105</v>
+        <v>1.049698033468303</v>
       </c>
       <c r="C26">
-        <v>-0.5887246149933119</v>
+        <v>0.5431833854864841</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1782,10 +1782,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-0.4497539711661407</v>
+        <v>1.302499141139639</v>
       </c>
       <c r="C27">
-        <v>0.3570254898020879</v>
+        <v>0.2419745310100135</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1793,10 +1793,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.09930555847055698</v>
+        <v>0.5981377106559861</v>
       </c>
       <c r="C28">
-        <v>-1.967798259232585</v>
+        <v>0.3378305810398273</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1804,10 +1804,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1.221349721941697</v>
+        <v>0.271490136353227</v>
       </c>
       <c r="C29">
-        <v>-0.0637639601125688</v>
+        <v>-1.429502752229888</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1815,10 +1815,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-0.5413496278113928</v>
+        <v>-0.6604201317481259</v>
       </c>
       <c r="C30">
-        <v>1.974900746225193</v>
+        <v>0.87697278767048</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1826,10 +1826,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.7285246739846452</v>
+        <v>-1.833246096336599</v>
       </c>
       <c r="C31">
-        <v>0.6885099848135122</v>
+        <v>1.830184171056839</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1837,10 +1837,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-0.8233661024595778</v>
+        <v>-0.1194446008378872</v>
       </c>
       <c r="C32">
-        <v>1.671932443213848</v>
+        <v>-0.8296854637853195</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1848,10 +1848,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1.68904819148525</v>
+        <v>-1.403755047936611</v>
       </c>
       <c r="C33">
-        <v>0.60571769709623</v>
+        <v>0.6325102522582333</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1859,10 +1859,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.2721794908463546</v>
+        <v>0.755261757469209</v>
       </c>
       <c r="C34">
-        <v>-0.2306472214051058</v>
+        <v>-0.0009800446630148472</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1870,10 +1870,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-0.2601672164150087</v>
+        <v>0.05466183204124758</v>
       </c>
       <c r="C35">
-        <v>-0.1315691776565173</v>
+        <v>0.9764544594614774</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1881,10 +1881,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-0.1712485496528555</v>
+        <v>-1.439140242772982</v>
       </c>
       <c r="C36">
-        <v>0.989409298983579</v>
+        <v>0.2658620767454772</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1892,10 +1892,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-0.7613689835568339</v>
+        <v>-0.6188016485141874</v>
       </c>
       <c r="C37">
-        <v>-2.659519782392611</v>
+        <v>-0.1542412130922351</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1903,10 +1903,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2.082574021217494</v>
+        <v>-0.9065641081416944</v>
       </c>
       <c r="C38">
-        <v>0.2437756003790464</v>
+        <v>0.09849924825570704</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1914,10 +1914,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-0.9366602311380052</v>
+        <v>1.8730419003978</v>
       </c>
       <c r="C39">
-        <v>-0.8390051861443532</v>
+        <v>0.8460741311283735</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1925,10 +1925,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1.234569252460236</v>
+        <v>-0.003917778619547748</v>
       </c>
       <c r="C40">
-        <v>2.145714976302813</v>
+        <v>0.4654316113958095</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1936,10 +1936,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.2183450420794161</v>
+        <v>-0.5746793177616006</v>
       </c>
       <c r="C41">
-        <v>-0.4722877830928376</v>
+        <v>0.2460196716699576</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1947,10 +1947,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.6817591028178599</v>
+        <v>-1.281709021113018</v>
       </c>
       <c r="C42">
-        <v>-1.742348152735209</v>
+        <v>-0.2922875756581422</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1958,10 +1958,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-0.8519296539370911</v>
+        <v>-0.5099091349101297</v>
       </c>
       <c r="C43">
-        <v>-1.089292612436668</v>
+        <v>0.3551881216036321</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1969,10 +1969,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.3715529300237652</v>
+        <v>2.156876539855145</v>
       </c>
       <c r="C44">
-        <v>0.09627209626358654</v>
+        <v>0.01471333943230888</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1980,10 +1980,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.5027519162727737</v>
+        <v>-0.2274977745228388</v>
       </c>
       <c r="C45">
-        <v>0.389260012134693</v>
+        <v>0.9751775118699075</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1991,10 +1991,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>1.269605401045758</v>
+        <v>0.9358053671640869</v>
       </c>
       <c r="C46">
-        <v>-0.04314534434322178</v>
+        <v>0.4743102637281847</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2002,10 +2002,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.2121068639568153</v>
+        <v>-0.3447974902068832</v>
       </c>
       <c r="C47">
-        <v>0.2800621734971939</v>
+        <v>-0.5055410197431597</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2013,10 +2013,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.3115035384227927</v>
+        <v>0.8102855503885027</v>
       </c>
       <c r="C48">
-        <v>1.294933872939559</v>
+        <v>0.6976734840309503</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2024,10 +2024,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.02924754490574958</v>
+        <v>2.732017126720732</v>
       </c>
       <c r="C49">
-        <v>-0.6270845202087074</v>
+        <v>0.4209881714830574</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2035,10 +2035,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.6596379489275901</v>
+        <v>-1.481287607705471</v>
       </c>
       <c r="C50">
-        <v>0.5540597602516814</v>
+        <v>0.2068318257361759</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2046,10 +2046,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.140498715582958</v>
+        <v>-0.2373617799508041</v>
       </c>
       <c r="C51">
-        <v>0.805437492618439</v>
+        <v>1.093238316293554</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2057,10 +2057,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>-1.46959638781043</v>
+        <v>-1.54956208507839</v>
       </c>
       <c r="C52">
-        <v>-0.3858804821313245</v>
+        <v>-1.007458535687109</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2068,10 +2068,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>-1.553425486455735</v>
+        <v>0.04210623463414916</v>
       </c>
       <c r="C53">
-        <v>0.9669320420337171</v>
+        <v>1.900553891081147</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2079,10 +2079,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1.102324214923103</v>
+        <v>1.106066249031037</v>
       </c>
       <c r="C54">
-        <v>-0.9583643141345461</v>
+        <v>0.6330632129040724</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2090,10 +2090,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.1718518924178439</v>
+        <v>-0.3755492325763147</v>
       </c>
       <c r="C55">
-        <v>-0.8734694915795295</v>
+        <v>-1.724103916176558</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2101,10 +2101,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.5525811757445014</v>
+        <v>-0.6326883428057873</v>
       </c>
       <c r="C56">
-        <v>0.4051268820548231</v>
+        <v>1.260719207934761</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2112,10 +2112,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1.42548859601397</v>
+        <v>-1.230451127673553</v>
       </c>
       <c r="C57">
-        <v>0.4626270561113193</v>
+        <v>1.815848526439576</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2123,10 +2123,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>-0.2136929637645566</v>
+        <v>-0.6343662623507739</v>
       </c>
       <c r="C58">
-        <v>-0.5088745940660754</v>
+        <v>0.740857308118788</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2134,10 +2134,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-2.021238660617388</v>
+        <v>-0.08900206385252739</v>
       </c>
       <c r="C59">
-        <v>-0.3908029775933578</v>
+        <v>-0.4893906338820531</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2145,10 +2145,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.8621684612545391</v>
+        <v>-0.2205669866777333</v>
       </c>
       <c r="C60">
-        <v>0.589728032059483</v>
+        <v>-0.7254149468221853</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2156,10 +2156,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>1.289319622463053</v>
+        <v>0.7400027493427466</v>
       </c>
       <c r="C61">
-        <v>-2.550818233923102</v>
+        <v>0.2454393937833157</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2167,10 +2167,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.5746756782034249</v>
+        <v>-0.4352752027077238</v>
       </c>
       <c r="C62">
-        <v>0.3713116050196777</v>
+        <v>0.8738843205854299</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2178,10 +2178,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.0502518755789016</v>
+        <v>1.272567391509297</v>
       </c>
       <c r="C63">
-        <v>-0.7289294872029346</v>
+        <v>0.9713454205131548</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2189,10 +2189,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.7186725301061901</v>
+        <v>1.023093964086024</v>
       </c>
       <c r="C64">
-        <v>1.282192230695511</v>
+        <v>0.5923800222623211</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2200,10 +2200,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.7560042908047344</v>
+        <v>0.9227212165546715</v>
       </c>
       <c r="C65">
-        <v>-0.341437729735685</v>
+        <v>0.8990875450224115</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2211,10 +2211,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-0.4149310813400631</v>
+        <v>3.187003945307631</v>
       </c>
       <c r="C66">
-        <v>1.199646645039128</v>
+        <v>0.6589457411383732</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2222,10 +2222,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-0.5766868681149088</v>
+        <v>2.933017819675014</v>
       </c>
       <c r="C67">
-        <v>-1.843270930960343</v>
+        <v>1.16124068144887</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2233,10 +2233,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>-0.5337924808916802</v>
+        <v>0.008228867749624802</v>
       </c>
       <c r="C68">
-        <v>1.419467788080163</v>
+        <v>0.9468593859405309</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2244,10 +2244,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>1.865738422278617</v>
+        <v>1.752863331958491</v>
       </c>
       <c r="C69">
-        <v>0.4374391208980958</v>
+        <v>-0.2132320664740931</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2255,10 +2255,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>1.273579203123053</v>
+        <v>1.285201118173074</v>
       </c>
       <c r="C70">
-        <v>1.162796766870934</v>
+        <v>-0.3411798483193713</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2266,10 +2266,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>-1.021613339639187</v>
+        <v>-0.3154736493830692</v>
       </c>
       <c r="C71">
-        <v>0.3236905371784118</v>
+        <v>0.9866472063630689</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2277,10 +2277,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>-0.113698373720609</v>
+        <v>-0.6337689394807939</v>
       </c>
       <c r="C72">
-        <v>-1.188709314802791</v>
+        <v>1.531101448345485</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2288,10 +2288,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>-0.05061213496173492</v>
+        <v>0.2651550333251318</v>
       </c>
       <c r="C73">
-        <v>0.122495289525486</v>
+        <v>1.559658431070031</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2299,10 +2299,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>1.218244905341852</v>
+        <v>0.1872997526973422</v>
       </c>
       <c r="C74">
-        <v>-0.6349390877949492</v>
+        <v>-0.2466986571864988</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2310,10 +2310,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>2.832343674446302</v>
+        <v>2.451830903512643</v>
       </c>
       <c r="C75">
-        <v>0.4084389489865016</v>
+        <v>0.5332391879809889</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2321,10 +2321,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.1229970054385632</v>
+        <v>-0.4756884755098194</v>
       </c>
       <c r="C76">
-        <v>1.153950725097825</v>
+        <v>-2.354511389150562</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2332,10 +2332,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>-0.7406658651481856</v>
+        <v>0.154461080228748</v>
       </c>
       <c r="C77">
-        <v>-0.7081382783035773</v>
+        <v>-1.640994596724842</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2343,10 +2343,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>-0.02803944908343457</v>
+        <v>-1.828783702619473</v>
       </c>
       <c r="C78">
-        <v>0.3110954786527377</v>
+        <v>0.3498422223650346</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2354,10 +2354,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>-0.5945383459963437</v>
+        <v>0.5604316865191199</v>
       </c>
       <c r="C79">
-        <v>-1.123078280366824</v>
+        <v>0.7358888902569546</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2365,10 +2365,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>1.141890021998772</v>
+        <v>-0.6401429203073166</v>
       </c>
       <c r="C80">
-        <v>1.574689499735958</v>
+        <v>-1.415202937860237</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2376,10 +2376,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.209459596017263</v>
+        <v>-2.136267171940676</v>
       </c>
       <c r="C81">
-        <v>0.9223098168568068</v>
+        <v>-0.7901796889360349</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2387,10 +2387,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-1.878361801422561</v>
+        <v>1.515104387165458</v>
       </c>
       <c r="C82">
-        <v>-0.3180707281504346</v>
+        <v>0.6682648725172098</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2398,10 +2398,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-0.352579926272619</v>
+        <v>-0.4374995114141306</v>
       </c>
       <c r="C83">
-        <v>-0.5943008564168779</v>
+        <v>-1.923716795245491</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2409,10 +2409,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>1.026061221965542</v>
+        <v>0.5939927086245168</v>
       </c>
       <c r="C84">
-        <v>0.5899914985605773</v>
+        <v>0.4102438283422876</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2420,10 +2420,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-0.4639971575021435</v>
+        <v>0.448994451571917</v>
       </c>
       <c r="C85">
-        <v>0.3044447880917853</v>
+        <v>1.01695508869954</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2431,10 +2431,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.8971280126409111</v>
+        <v>1.633079679120075</v>
       </c>
       <c r="C86">
-        <v>0.2005538522429882</v>
+        <v>-0.5542927483384702</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2442,10 +2442,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.1987810845460715</v>
+        <v>-0.3908248157174969</v>
       </c>
       <c r="C87">
-        <v>-0.6998699734933873</v>
+        <v>-0.5233546252828485</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2453,10 +2453,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>-1.081263154959099</v>
+        <v>0.2595001950005325</v>
       </c>
       <c r="C88">
-        <v>-1.366630253053152</v>
+        <v>1.430258011502492</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2464,10 +2464,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>-0.2855616255715158</v>
+        <v>0.2157158672040455</v>
       </c>
       <c r="C89">
-        <v>0.1389572001155436</v>
+        <v>-0.7478232182979032</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2475,10 +2475,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>1.158792121980529</v>
+        <v>0.1878961303097193</v>
       </c>
       <c r="C90">
-        <v>-0.8465840710751262</v>
+        <v>-0.8307693486456922</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2486,10 +2486,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.2597632737917488</v>
+        <v>0.08954575006630955</v>
       </c>
       <c r="C91">
-        <v>0.8153854020693539</v>
+        <v>-1.608726671336599</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2497,10 +2497,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>-0.4360405440420972</v>
+        <v>-0.6055187808239338</v>
       </c>
       <c r="C92">
-        <v>0.1193779292461118</v>
+        <v>-1.768933128321152</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2508,10 +2508,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>-0.3686773638261752</v>
+        <v>1.041671334929855</v>
       </c>
       <c r="C93">
-        <v>-0.736392978943639</v>
+        <v>0.5025018986441411</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2519,10 +2519,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.5331055216283129</v>
+        <v>0.03220992006580174</v>
       </c>
       <c r="C94">
-        <v>-1.189850013654858</v>
+        <v>-2.044313594589525</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2530,10 +2530,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>-1.605595062561054</v>
+        <v>-0.4669524915728909</v>
       </c>
       <c r="C95">
-        <v>1.187670497149707</v>
+        <v>-1.990844805001939</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2541,10 +2541,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.0565147346421365</v>
+        <v>-1.103705625399801</v>
       </c>
       <c r="C96">
-        <v>0.5336974237463713</v>
+        <v>0.39153116317902</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2552,10 +2552,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-2.46845528176494</v>
+        <v>-0.5524511890103677</v>
       </c>
       <c r="C97">
-        <v>0.2606844293699421</v>
+        <v>0.4071228701456703</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2563,10 +2563,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-0.7265914210120417</v>
+        <v>0.1452467142520832</v>
       </c>
       <c r="C98">
-        <v>0.9719646960608099</v>
+        <v>-0.2468653391905227</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2574,10 +2574,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>-1.086182303643217</v>
+        <v>-0.9586024734149173</v>
       </c>
       <c r="C99">
-        <v>0.9485624610215116</v>
+        <v>1.952078469304985</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2585,10 +2585,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>-1.189031271729276</v>
+        <v>0.6891972536822433</v>
       </c>
       <c r="C100">
-        <v>0.7843198812714807</v>
+        <v>-0.3689784571680829</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2596,10 +2596,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-1.921531663669727</v>
+        <v>0.2303170767222976</v>
       </c>
       <c r="C101">
-        <v>0.1742121799748179</v>
+        <v>0.3533459810969955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>